<commit_message>
feat: implement unified master database spreadsheet system
- Added export function to download entire database as master spreadsheet
- Simplified import to single file upload with update_mode column
- Removed separate plants/inventory file uploads
- Each row controls its own action: add_new, update_existing, or archive
- Master spreadsheet includes all plant and inventory data in one file
- Export-edit-import workflow ensures data consistency

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/templates/plants_template.xlsx
+++ b/public/templates/plants_template.xlsx
@@ -66,13 +66,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -449,7 +452,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
@@ -489,162 +492,167 @@
           <t>plant_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>update_mode</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>latinname</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>commonname</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>featured</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>height_inches</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>spread_inches</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>sunlight</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>hardiness_zones</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>bloom_season</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>colour</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>special_features</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>uses</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>aroma</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>gardening_tips</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>care_tips</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>mainimage</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>main_credit_type</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>main_credit_source</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>main_credit_photographer</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>main_credit_watermarked</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>additionalimage1</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>add1_credit_type</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>add1_credit_source</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>additionalimage2</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>add2_credit_type</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>add2_credit_source</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>additionalimage3</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>add3_credit_type</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>add3_credit_source</t>
         </is>
@@ -658,160 +666,165 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
+          <t>Update Mode</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Latin Name</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Common Name</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Featured</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>Height (inches)</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>Spread (inches)</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>Sunlight</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="L2" s="2" t="inlineStr">
         <is>
           <t>Hardiness Zones</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="M2" s="2" t="inlineStr">
         <is>
           <t>Bloom Season</t>
         </is>
       </c>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="N2" s="2" t="inlineStr">
         <is>
           <t>Colour</t>
         </is>
       </c>
-      <c r="N2" s="2" t="inlineStr">
+      <c r="O2" s="2" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="O2" s="2" t="inlineStr">
+      <c r="P2" s="2" t="inlineStr">
         <is>
           <t>Special Features</t>
         </is>
       </c>
-      <c r="P2" s="2" t="inlineStr">
+      <c r="Q2" s="2" t="inlineStr">
         <is>
           <t>Uses</t>
         </is>
       </c>
-      <c r="Q2" s="2" t="inlineStr">
+      <c r="R2" s="2" t="inlineStr">
         <is>
           <t>Aroma</t>
         </is>
       </c>
-      <c r="R2" s="2" t="inlineStr">
+      <c r="S2" s="2" t="inlineStr">
         <is>
           <t>Gardening Tips</t>
         </is>
       </c>
-      <c r="S2" s="2" t="inlineStr">
+      <c r="T2" s="2" t="inlineStr">
         <is>
           <t>Care Tips</t>
         </is>
       </c>
-      <c r="T2" s="2" t="inlineStr">
+      <c r="U2" s="2" t="inlineStr">
         <is>
           <t>Main Image URL</t>
         </is>
       </c>
-      <c r="U2" s="2" t="inlineStr">
+      <c r="V2" s="2" t="inlineStr">
         <is>
           <t>Main Image Credit Type</t>
         </is>
       </c>
-      <c r="V2" s="2" t="inlineStr">
+      <c r="W2" s="2" t="inlineStr">
         <is>
           <t>Main Image Source</t>
         </is>
       </c>
-      <c r="W2" s="2" t="inlineStr">
+      <c r="X2" s="2" t="inlineStr">
         <is>
           <t>Main Image Photographer</t>
         </is>
       </c>
-      <c r="X2" s="2" t="inlineStr">
+      <c r="Y2" s="2" t="inlineStr">
         <is>
           <t>Main Image Watermark</t>
         </is>
       </c>
-      <c r="Y2" s="2" t="inlineStr">
+      <c r="Z2" s="2" t="inlineStr">
         <is>
           <t>Additional Image 1 URL</t>
         </is>
       </c>
-      <c r="Z2" s="2" t="inlineStr">
+      <c r="AA2" s="2" t="inlineStr">
         <is>
           <t>Add Image 1 Credit Type</t>
         </is>
       </c>
-      <c r="AA2" s="2" t="inlineStr">
+      <c r="AB2" s="2" t="inlineStr">
         <is>
           <t>Add Image 1 Source</t>
         </is>
       </c>
-      <c r="AB2" s="2" t="inlineStr">
+      <c r="AC2" s="2" t="inlineStr">
         <is>
           <t>Additional Image 2 URL</t>
         </is>
       </c>
-      <c r="AC2" s="2" t="inlineStr">
+      <c r="AD2" s="2" t="inlineStr">
         <is>
           <t>Add Image 2 Credit Type</t>
         </is>
       </c>
-      <c r="AD2" s="2" t="inlineStr">
+      <c r="AE2" s="2" t="inlineStr">
         <is>
           <t>Add Image 2 Source</t>
         </is>
       </c>
-      <c r="AE2" s="2" t="inlineStr">
+      <c r="AF2" s="2" t="inlineStr">
         <is>
           <t>Additional Image 3 URL</t>
         </is>
       </c>
-      <c r="AF2" s="2" t="inlineStr">
+      <c r="AG2" s="2" t="inlineStr">
         <is>
           <t>Add Image 3 Credit Type</t>
         </is>
       </c>
-      <c r="AG2" s="2" t="inlineStr">
+      <c r="AH2" s="2" t="inlineStr">
         <is>
           <t>Add Image 3 Source</t>
         </is>
@@ -825,147 +838,152 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Example Rose</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Rosa example</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Garden Rose</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>12.99</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Perennial</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Full Sun</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>5-9</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Summer</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Beautiful example rose for testing</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>Fragrant, Long blooming</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Borders, Cut flowers</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>Strong</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>Plant in spring</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>Water regularly</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>https://firebasestorage.googleapis.com/v0/b/example/rose-main.jpg</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>commercial</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>Van Noort</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>https://firebasestorage.googleapis.com/v0/b/example/rose-1.jpg</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>own</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>Button's Flower Farm</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>https://firebasestorage.googleapis.com/v0/b/example/rose-2.jpg</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AD3" t="inlineStr">
         <is>
           <t>commercial</t>
         </is>
       </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AE3" t="inlineStr">
         <is>
           <t>Jelitto</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation sqref="U3:U1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid entry" error="Please select: own, commercial, or none" type="list">
       <formula1>"own,commercial,none"</formula1>
     </dataValidation>
@@ -981,6 +999,9 @@
     <dataValidation sqref="X3:X1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid entry" error="Please select YES or NO" type="list">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
+    <dataValidation sqref="B3:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Mode" error="Please select: add, update, or archive" type="list">
+      <formula1>"add,update,archive"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>